<commit_message>
added 3 more stars and stopped key controls from bubbling up while typing
</commit_message>
<xml_diff>
--- a/data/StarDatabaseOngoing.xlsx
+++ b/data/StarDatabaseOngoing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Desktop\Projects\StarJourney\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Documents\Projects\StarJourney\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CDBE751D-6B98-42DA-9F5E-B7D619A4748D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86F926C-3DE9-46E6-A812-0CBD0A9D24A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{0FF2E678-94B6-4BC7-828A-6A66D6B612B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{0FF2E678-94B6-4BC7-828A-6A66D6B612B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -235,6 +235,63 @@
   </si>
   <si>
     <t>Color Index (B-V)</t>
+  </si>
+  <si>
+    <t>Gl 905</t>
+  </si>
+  <si>
+    <t>Andromeda</t>
+  </si>
+  <si>
+    <t>M6V</t>
+  </si>
+  <si>
+    <t>Ross 248</t>
+  </si>
+  <si>
+    <t>HH Andromedae</t>
+  </si>
+  <si>
+    <t>Epsilon Eridani</t>
+  </si>
+  <si>
+    <t>Epsilon Eridani;Ran</t>
+  </si>
+  <si>
+    <t>Eridanus</t>
+  </si>
+  <si>
+    <t>K2V</t>
+  </si>
+  <si>
+    <t>Gl 144</t>
+  </si>
+  <si>
+    <t>Approx Color</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>Lacaille 9352</t>
+  </si>
+  <si>
+    <t>Gl 887</t>
+  </si>
+  <si>
+    <t>M0.5V</t>
+  </si>
+  <si>
+    <t>Piscus Austrinus</t>
   </si>
 </sst>
 </file>
@@ -586,18 +643,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F71653-5046-4143-AD34-6664A35D7840}">
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,31 +713,34 @@
         <v>15</v>
       </c>
       <c r="T1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>6</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>11</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -732,8 +792,11 @@
       <c r="R2">
         <v>0.65600000000000003</v>
       </c>
+      <c r="T2" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -774,13 +837,16 @@
         <v>1.8069999999999999</v>
       </c>
       <c r="T3" t="s">
+        <v>81</v>
+      </c>
+      <c r="U3" t="s">
         <v>38</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>70890</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -821,22 +887,25 @@
         <v>0.71</v>
       </c>
       <c r="T4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U4" t="s">
         <v>38</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>128620</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>25</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>71683</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>5459</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -877,22 +946,25 @@
         <v>0.9</v>
       </c>
       <c r="T5" t="s">
+        <v>82</v>
+      </c>
+      <c r="U5" t="s">
         <v>38</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>128621</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>26</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>71681</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>5460</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -933,13 +1005,16 @@
         <v>1.57</v>
       </c>
       <c r="T6" t="s">
+        <v>81</v>
+      </c>
+      <c r="U6" t="s">
         <v>60</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>87937</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -980,10 +1055,13 @@
         <v>2</v>
       </c>
       <c r="T7" t="s">
+        <v>81</v>
+      </c>
+      <c r="U7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1024,16 +1102,19 @@
         <v>1.502</v>
       </c>
       <c r="T8" t="s">
+        <v>81</v>
+      </c>
+      <c r="U8" t="s">
         <v>46</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>95735</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>54035</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1074,10 +1155,13 @@
         <v>1.85</v>
       </c>
       <c r="T9" t="s">
+        <v>84</v>
+      </c>
+      <c r="U9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1118,10 +1202,13 @@
         <v>1.87</v>
       </c>
       <c r="T10" t="s">
+        <v>84</v>
+      </c>
+      <c r="U10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1162,22 +1249,25 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="T11" t="s">
+        <v>83</v>
+      </c>
+      <c r="U11" t="s">
         <v>47</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>48915</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>65</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>9</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>32349</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1218,13 +1308,16 @@
         <v>-0.03</v>
       </c>
       <c r="T12" t="s">
+        <v>84</v>
+      </c>
+      <c r="U12" t="s">
         <v>47</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1265,10 +1358,178 @@
         <v>1.51</v>
       </c>
       <c r="T13" t="s">
+        <v>81</v>
+      </c>
+      <c r="U13" t="s">
         <v>48</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>92403</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14">
+        <v>3.1549282999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.16</v>
+      </c>
+      <c r="F14">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G14">
+        <v>23.698378999999999</v>
+      </c>
+      <c r="H14">
+        <v>44.174923999999997</v>
+      </c>
+      <c r="N14">
+        <v>12.3</v>
+      </c>
+      <c r="O14">
+        <v>14.79</v>
+      </c>
+      <c r="P14">
+        <v>1.8E-3</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14">
+        <v>1.92</v>
+      </c>
+      <c r="T14" t="s">
+        <v>81</v>
+      </c>
+      <c r="U14" t="s">
+        <v>71</v>
+      </c>
+      <c r="W14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15">
+        <v>3.2116495999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.82</v>
+      </c>
+      <c r="G15">
+        <v>3.548848</v>
+      </c>
+      <c r="H15">
+        <v>-9.4582619999999995</v>
+      </c>
+      <c r="N15">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="O15">
+        <v>6.19</v>
+      </c>
+      <c r="P15">
+        <v>0.34</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R15">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="T15" t="s">
+        <v>82</v>
+      </c>
+      <c r="U15" t="s">
+        <v>77</v>
+      </c>
+      <c r="V15">
+        <v>22049</v>
+      </c>
+      <c r="W15" t="s">
+        <v>75</v>
+      </c>
+      <c r="X15">
+        <v>18</v>
+      </c>
+      <c r="Y15">
+        <v>16537</v>
+      </c>
+      <c r="AA15">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16">
+        <v>3.2745028999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.503</v>
+      </c>
+      <c r="F16">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="G16">
+        <v>23.097531</v>
+      </c>
+      <c r="H16">
+        <v>-35.853073000000002</v>
+      </c>
+      <c r="N16">
+        <v>7.34</v>
+      </c>
+      <c r="O16">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="P16">
+        <v>0.33</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>87</v>
+      </c>
+      <c r="R16">
+        <v>1.5</v>
+      </c>
+      <c r="T16" t="s">
+        <v>81</v>
+      </c>
+      <c r="U16" t="s">
+        <v>88</v>
+      </c>
+      <c r="V16">
+        <v>217987</v>
+      </c>
+      <c r="Y16">
+        <v>114046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added inhereted classes for stars and planets, and a sample data view
</commit_message>
<xml_diff>
--- a/data/StarDatabaseOngoing.xlsx
+++ b/data/StarDatabaseOngoing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Documents\Projects\StarJourney\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86F926C-3DE9-46E6-A812-0CBD0A9D24A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB12614-C932-4DBA-A124-355BD2718840}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{0FF2E678-94B6-4BC7-828A-6A66D6B612B4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Piscus Austrinus</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F71653-5046-4143-AD34-6664A35D7840}">
-  <dimension ref="A1:AB16"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +657,7 @@
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,8 +742,11 @@
       <c r="AB1" t="s">
         <v>57</v>
       </c>
+      <c r="AC1" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -796,7 +802,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -846,7 +852,7 @@
         <v>70890</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -905,7 +911,7 @@
         <v>5459</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -964,7 +970,7 @@
         <v>5460</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>87937</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>54035</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1267,7 +1273,7 @@
         <v>32349</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>92403</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1417,7 +1423,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
small update to star database
</commit_message>
<xml_diff>
--- a/data/StarDatabaseOngoing.xlsx
+++ b/data/StarDatabaseOngoing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Documents\Projects\StarJourney\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Documents\Projects\StarJourney\StarJourney\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB12614-C932-4DBA-A124-355BD2718840}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D42B4D-BC08-43F4-80B5-2E1487103172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{0FF2E678-94B6-4BC7-828A-6A66D6B612B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FF2E678-94B6-4BC7-828A-6A66D6B612B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -295,6 +295,141 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Gl 447</t>
+  </si>
+  <si>
+    <t>Gl 866A</t>
+  </si>
+  <si>
+    <t>Gl 725B</t>
+  </si>
+  <si>
+    <t>Gl 820A</t>
+  </si>
+  <si>
+    <t>Gl 280B</t>
+  </si>
+  <si>
+    <t>Gl 820B</t>
+  </si>
+  <si>
+    <t>Gl 280A</t>
+  </si>
+  <si>
+    <t>Gl 15B</t>
+  </si>
+  <si>
+    <t>Gl 725A</t>
+  </si>
+  <si>
+    <t>Gl 15A</t>
+  </si>
+  <si>
+    <t>Gl 845</t>
+  </si>
+  <si>
+    <t>GJ 1111</t>
+  </si>
+  <si>
+    <t>Gl 71</t>
+  </si>
+  <si>
+    <t>Gl 54.1</t>
+  </si>
+  <si>
+    <t>Gl 273</t>
+  </si>
+  <si>
+    <t>Gl 191</t>
+  </si>
+  <si>
+    <t>Gl 825</t>
+  </si>
+  <si>
+    <t>Gl 860A</t>
+  </si>
+  <si>
+    <t>Gl 860B</t>
+  </si>
+  <si>
+    <t>Gl 563.2B</t>
+  </si>
+  <si>
+    <t>Gl 234B</t>
+  </si>
+  <si>
+    <t>Gl 234A</t>
+  </si>
+  <si>
+    <t>Gl 35</t>
+  </si>
+  <si>
+    <t>GJ 1061</t>
+  </si>
+  <si>
+    <t>Gl 628</t>
+  </si>
+  <si>
+    <t>Gl 473A</t>
+  </si>
+  <si>
+    <t>Gl 473B</t>
+  </si>
+  <si>
+    <t>Gl 1</t>
+  </si>
+  <si>
+    <t>NN 3522</t>
+  </si>
+  <si>
+    <t>Gl 83.1</t>
+  </si>
+  <si>
+    <t>NN 3618</t>
+  </si>
+  <si>
+    <t>NN 3622</t>
+  </si>
+  <si>
+    <t>Gl 687</t>
+  </si>
+  <si>
+    <t>Gl 674</t>
+  </si>
+  <si>
+    <t>Procyon</t>
+  </si>
+  <si>
+    <t>Ross 128</t>
+  </si>
+  <si>
+    <t>Virgo</t>
+  </si>
+  <si>
+    <t>M4V</t>
+  </si>
+  <si>
+    <t>M5e</t>
+  </si>
+  <si>
+    <t>Aquarius</t>
+  </si>
+  <si>
+    <t>Gl 866B</t>
+  </si>
+  <si>
+    <t>EZ Aquarii A</t>
+  </si>
+  <si>
+    <t>EZ Aquarii B</t>
+  </si>
+  <si>
+    <t>EZ Aquarii C</t>
+  </si>
+  <si>
+    <t>orbits as the companion to the other two's primary</t>
   </si>
 </sst>
 </file>
@@ -646,15 +781,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F71653-5046-4143-AD34-6664A35D7840}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AC54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -1538,6 +1675,775 @@
         <v>114046</v>
       </c>
     </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>3.3553000000000002</v>
+      </c>
+      <c r="E17">
+        <v>0.19670000000000001</v>
+      </c>
+      <c r="F17">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G17">
+        <v>11.795666000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.80456300000000003</v>
+      </c>
+      <c r="N17">
+        <v>11.13</v>
+      </c>
+      <c r="O17">
+        <v>13.53</v>
+      </c>
+      <c r="P17">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>127</v>
+      </c>
+      <c r="R17">
+        <v>1.59</v>
+      </c>
+      <c r="T17" t="s">
+        <v>81</v>
+      </c>
+      <c r="U17" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y17">
+        <v>57548</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>3.3978999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.35</v>
+      </c>
+      <c r="F18">
+        <v>0.11</v>
+      </c>
+      <c r="G18">
+        <v>22.642562000000002</v>
+      </c>
+      <c r="H18">
+        <v>-15.302542000000001</v>
+      </c>
+      <c r="N18">
+        <v>13.33</v>
+      </c>
+      <c r="O18">
+        <v>15.64</v>
+      </c>
+      <c r="P18">
+        <v>8.7000000000000001E-5</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>128</v>
+      </c>
+      <c r="R18">
+        <v>1.96</v>
+      </c>
+      <c r="T18" t="s">
+        <v>81</v>
+      </c>
+      <c r="U18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19">
+        <v>3.3978999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.35</v>
+      </c>
+      <c r="F19">
+        <v>0.11</v>
+      </c>
+      <c r="G19">
+        <v>22.642562000000002</v>
+      </c>
+      <c r="H19">
+        <v>-15.302542000000001</v>
+      </c>
+      <c r="N19">
+        <v>13.27</v>
+      </c>
+      <c r="O19">
+        <v>15.58</v>
+      </c>
+      <c r="P19">
+        <v>3.4E-5</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>128</v>
+      </c>
+      <c r="R19">
+        <v>1.96</v>
+      </c>
+      <c r="T19" t="s">
+        <v>81</v>
+      </c>
+      <c r="U19" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20">
+        <v>3.3978999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.35</v>
+      </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
+      <c r="G20">
+        <v>22.642562000000002</v>
+      </c>
+      <c r="H20">
+        <v>-15.302542000000001</v>
+      </c>
+      <c r="N20">
+        <v>14.03</v>
+      </c>
+      <c r="O20">
+        <v>16.34</v>
+      </c>
+      <c r="P20">
+        <v>2.2909999999999999E-5</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>128</v>
+      </c>
+      <c r="R20">
+        <v>1.96</v>
+      </c>
+      <c r="T20" t="s">
+        <v>81</v>
+      </c>
+      <c r="U20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21">
+        <v>3.4544999999999999</v>
+      </c>
+      <c r="G21">
+        <v>18.713249000000001</v>
+      </c>
+      <c r="H21">
+        <v>59.626846999999998</v>
+      </c>
+      <c r="V21">
+        <v>173740</v>
+      </c>
+      <c r="Y21">
+        <v>91772</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22">
+        <v>3.4864999999999999</v>
+      </c>
+      <c r="G22">
+        <v>21.114794</v>
+      </c>
+      <c r="H22">
+        <v>38.749414999999999</v>
+      </c>
+      <c r="V22">
+        <v>201091</v>
+      </c>
+      <c r="Y22">
+        <v>104214</v>
+      </c>
+      <c r="AA22">
+        <v>8085</v>
+      </c>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23">
+        <v>3.4973999999999998</v>
+      </c>
+      <c r="G23">
+        <v>7.6550060000000002</v>
+      </c>
+      <c r="H23">
+        <v>5.2268239999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24">
+        <v>3.4980000000000002</v>
+      </c>
+      <c r="G24">
+        <v>21.115162999999999</v>
+      </c>
+      <c r="H24">
+        <v>38.742055000000001</v>
+      </c>
+      <c r="V24">
+        <v>201092</v>
+      </c>
+      <c r="Y24">
+        <v>104217</v>
+      </c>
+      <c r="AA24">
+        <v>8086</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25">
+        <v>3.5142000000000002</v>
+      </c>
+      <c r="G25">
+        <v>7.6550330000000004</v>
+      </c>
+      <c r="H25">
+        <v>5.2249930000000004</v>
+      </c>
+      <c r="V25">
+        <v>61421</v>
+      </c>
+      <c r="Y25">
+        <v>37279</v>
+      </c>
+      <c r="AA25">
+        <v>2943</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26">
+        <v>3.5680000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.30515999999999999</v>
+      </c>
+      <c r="H26">
+        <v>44.023502000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27">
+        <v>3.5691000000000002</v>
+      </c>
+      <c r="G27">
+        <v>18.713179</v>
+      </c>
+      <c r="H27">
+        <v>59.630395999999998</v>
+      </c>
+      <c r="V27">
+        <v>173739</v>
+      </c>
+      <c r="Y27">
+        <v>91768</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28">
+        <v>3.5872999999999999</v>
+      </c>
+      <c r="G28">
+        <v>0.306174</v>
+      </c>
+      <c r="H28">
+        <v>44.022953999999999</v>
+      </c>
+      <c r="V28">
+        <v>1326</v>
+      </c>
+      <c r="Y28">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29">
+        <v>3.6223999999999998</v>
+      </c>
+      <c r="G29">
+        <v>22.055485999999998</v>
+      </c>
+      <c r="H29">
+        <v>-56.785977000000003</v>
+      </c>
+      <c r="V29">
+        <v>209100</v>
+      </c>
+      <c r="Y29">
+        <v>108870</v>
+      </c>
+      <c r="AA29">
+        <v>8387</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30">
+        <v>3.6257999999999999</v>
+      </c>
+      <c r="G30">
+        <v>8.4972440000000002</v>
+      </c>
+      <c r="H30">
+        <v>26.778531999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31">
+        <v>3.6501999999999999</v>
+      </c>
+      <c r="G31">
+        <v>1.7344790000000001</v>
+      </c>
+      <c r="H31">
+        <v>-15.937480000000001</v>
+      </c>
+      <c r="V31">
+        <v>10700</v>
+      </c>
+      <c r="Y31">
+        <v>8102</v>
+      </c>
+      <c r="AA31">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32">
+        <v>3.6899000000000002</v>
+      </c>
+      <c r="G32">
+        <v>1.208502</v>
+      </c>
+      <c r="H32">
+        <v>-16.998967</v>
+      </c>
+      <c r="Y32">
+        <v>5643</v>
+      </c>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>3.6964000000000001</v>
+      </c>
+      <c r="G33">
+        <v>16.908863</v>
+      </c>
+      <c r="H33">
+        <v>-62.399734000000002</v>
+      </c>
+      <c r="Y33">
+        <v>82724</v>
+      </c>
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34">
+        <v>3.8026</v>
+      </c>
+      <c r="G34">
+        <v>7.4568050000000001</v>
+      </c>
+      <c r="H34">
+        <v>5.2257850000000001</v>
+      </c>
+      <c r="Y34">
+        <v>36208</v>
+      </c>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35">
+        <v>3.9114</v>
+      </c>
+      <c r="G35">
+        <v>5.1941689999999996</v>
+      </c>
+      <c r="H35">
+        <v>-45.018416999999999</v>
+      </c>
+      <c r="V35">
+        <v>33793</v>
+      </c>
+      <c r="Y35">
+        <v>24186</v>
+      </c>
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36">
+        <v>3.9462000000000002</v>
+      </c>
+      <c r="G36">
+        <v>21.287724999999998</v>
+      </c>
+      <c r="H36">
+        <v>-38.867362</v>
+      </c>
+      <c r="V36">
+        <v>202560</v>
+      </c>
+      <c r="Y36">
+        <v>105090</v>
+      </c>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37">
+        <v>4.0010000000000003</v>
+      </c>
+      <c r="G37">
+        <v>22.466642</v>
+      </c>
+      <c r="H37">
+        <v>57.695875000000001</v>
+      </c>
+      <c r="V37">
+        <v>239960</v>
+      </c>
+      <c r="Y37">
+        <v>110893</v>
+      </c>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38">
+        <v>4.0076999999999998</v>
+      </c>
+      <c r="G38">
+        <v>22.467267</v>
+      </c>
+      <c r="H38">
+        <v>57.696623000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39">
+        <v>4.0339999999999998</v>
+      </c>
+      <c r="G39">
+        <v>14.825751</v>
+      </c>
+      <c r="H39">
+        <v>-26.105703999999999</v>
+      </c>
+      <c r="Y39">
+        <v>72511</v>
+      </c>
+    </row>
+    <row r="40" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40">
+        <v>4.1170999999999998</v>
+      </c>
+      <c r="G40">
+        <v>6.4899389999999997</v>
+      </c>
+      <c r="H40">
+        <v>-2.812227</v>
+      </c>
+    </row>
+    <row r="41" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41">
+        <v>4.1268000000000002</v>
+      </c>
+      <c r="G41">
+        <v>6.489833</v>
+      </c>
+      <c r="H41">
+        <v>-2.8139789999999998</v>
+      </c>
+      <c r="Y41">
+        <v>30920</v>
+      </c>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>4.1464999999999996</v>
+      </c>
+      <c r="G42">
+        <v>16.908971000000001</v>
+      </c>
+      <c r="H42">
+        <v>-62.403319000000003</v>
+      </c>
+      <c r="Y42">
+        <v>82725</v>
+      </c>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43">
+        <v>4.2625999999999999</v>
+      </c>
+      <c r="G43">
+        <v>0.81941600000000003</v>
+      </c>
+      <c r="H43">
+        <v>5.3886099999999999</v>
+      </c>
+      <c r="Y43">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="44" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44">
+        <v>4.2918000000000003</v>
+      </c>
+      <c r="G44">
+        <v>3.599704</v>
+      </c>
+      <c r="H44">
+        <v>-44.511896999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45">
+        <v>4.2922000000000002</v>
+      </c>
+      <c r="G45">
+        <v>16.505016999999999</v>
+      </c>
+      <c r="H45">
+        <v>-12.662594</v>
+      </c>
+      <c r="Y45">
+        <v>80824</v>
+      </c>
+    </row>
+    <row r="46" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46">
+        <v>4.3066000000000004</v>
+      </c>
+      <c r="G46">
+        <v>12.554778000000001</v>
+      </c>
+      <c r="H46">
+        <v>9.0207139999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47">
+        <v>4.3066000000000004</v>
+      </c>
+      <c r="G47">
+        <v>12.554778000000001</v>
+      </c>
+      <c r="H47">
+        <v>9.0207139999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48">
+        <v>4.3399000000000001</v>
+      </c>
+      <c r="G48">
+        <v>8.9883000000000005E-2</v>
+      </c>
+      <c r="H48">
+        <v>-37.357363999999997</v>
+      </c>
+      <c r="V48">
+        <v>225213</v>
+      </c>
+      <c r="Y48">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="49" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49">
+        <v>4.4642999999999997</v>
+      </c>
+      <c r="G49">
+        <v>8.9822360000000003</v>
+      </c>
+      <c r="H49">
+        <v>8.4753969999999992</v>
+      </c>
+    </row>
+    <row r="50" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50">
+        <v>4.4683000000000002</v>
+      </c>
+      <c r="G50">
+        <v>2.0035630000000002</v>
+      </c>
+      <c r="H50">
+        <v>13.053039999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51">
+        <v>4.4882999999999997</v>
+      </c>
+      <c r="G51">
+        <v>10.742414</v>
+      </c>
+      <c r="H51">
+        <v>-61.193586000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D52">
+        <v>4.5248999999999997</v>
+      </c>
+      <c r="G52">
+        <v>10.803471</v>
+      </c>
+      <c r="H52">
+        <v>-11.336727</v>
+      </c>
+    </row>
+    <row r="53" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53">
+        <v>4.5282</v>
+      </c>
+      <c r="G53">
+        <v>17.607282999999999</v>
+      </c>
+      <c r="H53">
+        <v>68.339140999999998</v>
+      </c>
+      <c r="Y53">
+        <v>86162</v>
+      </c>
+    </row>
+    <row r="54" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54">
+        <v>4.5404999999999998</v>
+      </c>
+      <c r="G54">
+        <v>17.477720000000001</v>
+      </c>
+      <c r="H54">
+        <v>-46.895189999999999</v>
+      </c>
+      <c r="Y54">
+        <v>85523</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>